<commit_message>
Add INI functions, change log format, etc.
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5175" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5175"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="262">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,872 +147,880 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>INIRead</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INIDelete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INIAddSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INIDeleteSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INIWriteTextLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INIMerge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegHiveLoad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FileMove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB082</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineFile.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineRegistry.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineText.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegExport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHOW deprecated, not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GetParam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PackParam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Attach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExtractFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExtractAndRun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExtractAllFiles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ExtractAllFilesIfNotExist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebGet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WebGetIfNotExist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEnginePlugin.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Visible</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Message</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Echo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineNetwork.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddVariables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShellExecute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wait</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineUI.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,Dir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,File</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,FileSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,FileVersion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,FolderSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,MD5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineString.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StringFormat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,CharToOEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Floor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Ceil</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Bytes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,OEMToChar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated, not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,FileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Ext</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,DirPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Inc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Dec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Mult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Div</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat.Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Len</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,LTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,RTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,CTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,NTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,SubStr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,ShortPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,LongPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineSystem.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,GetEnv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,Cursor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,Log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RefreshInterface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,SaveLog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,SplitParameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RescanScript</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RegRedirect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,Comp80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,ErrorOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,FileRedirect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,GetFreeDrive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,GetFreeSpace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,HasUAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,IsAdmin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,IsTerminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery can work across with UAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,OnBuildExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,OnScriptExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,OnPluginExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery is .Net Application, works without WOW64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Branch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Begin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Equal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotEqual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Smaller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Bigger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,EqualX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Ping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Online</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,License</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistMacro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistRegMulti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extended</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== FIleRename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will be deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineBranch.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineControl.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,SHA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,SHA256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,SHA512</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MD5 is too old, isn’t it?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== C# String.IndexOf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== C# String.Split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>==System,OnScriptExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>==If,Not,Equal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>==If,Not,Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== StrFormat,DirPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TestSuite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>End</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Else</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implemented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,ReplaceX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Replace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== C# String.Replace, case insentitive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%BaseDir%</t>
+  </si>
+  <si>
+    <t>E:\WinPE\Win10PESE</t>
+  </si>
+  <si>
+    <t>%Build%</t>
+  </si>
+  <si>
+    <t>2011-Jul-01 12:16</t>
+  </si>
+  <si>
+    <t>%Day%</t>
+  </si>
+  <si>
+    <t>%DistLang%</t>
+  </si>
+  <si>
+    <t>ko-KR</t>
+  </si>
+  <si>
+    <t>%DistLangHost%</t>
+  </si>
+  <si>
+    <t>%FileVersion%</t>
+  </si>
+  <si>
+    <t>82.0.0.15</t>
+  </si>
+  <si>
+    <t>%GlobalSupport%</t>
+  </si>
+  <si>
+    <t>%BaseDir%\Workbench</t>
+  </si>
+  <si>
+    <t>%GlobalTemp%</t>
+  </si>
+  <si>
+    <t>%BaseDir%\Temp</t>
+  </si>
+  <si>
+    <t>%GlobalTemplates%</t>
+  </si>
+  <si>
+    <t>%Month%</t>
+  </si>
+  <si>
+    <t>%ProgramFilesDir%</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)</t>
+  </si>
+  <si>
+    <t>%Programs64%</t>
+  </si>
+  <si>
+    <t>C:\Program Files</t>
+  </si>
+  <si>
+    <t>%SourceArch%</t>
+  </si>
+  <si>
+    <t>x64</t>
+  </si>
+  <si>
+    <t>%SourceDir%</t>
+  </si>
+  <si>
+    <t>E:\WinPE\Source\Win10x64</t>
+  </si>
+  <si>
+    <t>%SystemDrive%</t>
+  </si>
+  <si>
+    <t>#$pSystemDrive#$p</t>
+  </si>
+  <si>
+    <t>%SysType%</t>
+  </si>
+  <si>
+    <t>X64</t>
+  </si>
+  <si>
+    <t>%TargetWOW64%</t>
+  </si>
+  <si>
+    <t>x86</t>
+  </si>
+  <si>
+    <t>%TempDir%</t>
+  </si>
+  <si>
+    <t>C:\Users\Joveler\AppData\Local\Temp</t>
+  </si>
+  <si>
+    <t>%UserName%</t>
+  </si>
+  <si>
+    <t>Joveler</t>
+  </si>
+  <si>
+    <t>%UserProfile%</t>
+  </si>
+  <si>
+    <t>C:\Users\Joveler</t>
+  </si>
+  <si>
+    <t>%Version%</t>
+  </si>
+  <si>
+    <t>%WBexe%</t>
+  </si>
+  <si>
+    <t>%BaseDir%\BuilderSE.exe</t>
+  </si>
+  <si>
+    <t>%WindowsDir%</t>
+  </si>
+  <si>
+    <t>C:\WINDOWS</t>
+  </si>
+  <si>
+    <t>%WindowsSystemDir%</t>
+  </si>
+  <si>
+    <t>C:\WINDOWS\system32</t>
+  </si>
+  <si>
+    <t>%Wow64%</t>
+  </si>
+  <si>
+    <t>%Wow64Dir%</t>
+  </si>
+  <si>
+    <t>C:\WINDOWS\SysWoW64</t>
+  </si>
+  <si>
+    <t>%Year%</t>
+  </si>
+  <si>
+    <t>Test Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Support</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB082 Test Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB082</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RebuildVars</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%BaseDir%\Workbench\Common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%ProcessorType%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%HostOS%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XP, W2003, WinVista</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Host OS's lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source media's lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default Global Variables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%ScriptFile%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%PluginFile%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;name of plugin&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreign plugin's section not implemented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>INIWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>INIRead</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INIDelete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INIAddSection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INIDeleteSection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INIWriteTextLine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INIMerge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CS File</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegHiveLoad</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FileMove</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WB082</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineFile.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineRegistry.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineText.cs</t>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery is new implementation of WinBuilder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unicode supported</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Encoding option added</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegExport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Need test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SHOW deprecated, not used in WinPESE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GetParam</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PackParam</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attach</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExtractFile</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExtractAndRun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExtractAllFiles</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ExtractAllFilesIfNotExist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Encode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Network</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WebGet</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WebGetIfNotExist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEnginePlugin.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Visible</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Message</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Echo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineNetwork.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AddVariables</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Beep</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Halt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShellExecute</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wait</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineUI.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,Dir</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,File</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,FileSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,FileVersion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,FolderSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,MD5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineString.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StringFormat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,CharToOEM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Floor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Ceil</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Bytes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,OEMToChar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated, not used in WinPESE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,FileName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Path</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Ext</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,DirPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Inc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Dec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Mult</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Div</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Left</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat.Right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Len</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,LTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,RTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,CTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,NTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Pos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,SubStr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,ShortPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,LongPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Split</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineSystem.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,GetEnv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,Cursor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,Log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RefreshInterface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,SaveLog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,SplitParameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RescanScript</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RegRedirect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,Comp80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,ErrorOff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,FileRedirect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,GetFreeDrive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,GetFreeSpace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,HasUAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,IsAdmin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,IsTerminal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery can work across with UAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,OnBuildExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,OnScriptExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,OnPluginExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery is .Net Application, works without WOW64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not used in WinPESE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Branch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Run</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,NotExist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Begin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Equal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,NotEqual</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Smaller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Bigger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,EqualX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Ping</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Online</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,License</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Not</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Question</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,ExistMacro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,ExistRegMulti</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extended</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>== FIleRename</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Will be deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineBranch.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Control</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineControl.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,SHA1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,SHA256</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,SHA512</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MD5 is too old, isn’t it?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Count</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>== C# String.IndexOf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>== C# String.Split</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery is new blackbox implementation of WinBuilder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>==System,OnScriptExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>==If,Not,Equal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>==If,Not,Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>== StrFormat,DirPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TestSuite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>End</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Else</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Implemented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Statistics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,ReplaceX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Replace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>== C# String.Replace, case insentitive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%BaseDir%</t>
-  </si>
-  <si>
-    <t>E:\WinPE\Win10PESE</t>
-  </si>
-  <si>
-    <t>%Build%</t>
-  </si>
-  <si>
-    <t>2011-Jul-01 12:16</t>
-  </si>
-  <si>
-    <t>%Day%</t>
-  </si>
-  <si>
-    <t>%DistLang%</t>
-  </si>
-  <si>
-    <t>ko-KR</t>
-  </si>
-  <si>
-    <t>%DistLangHost%</t>
-  </si>
-  <si>
-    <t>%FileVersion%</t>
-  </si>
-  <si>
-    <t>82.0.0.15</t>
-  </si>
-  <si>
-    <t>%GlobalSupport%</t>
-  </si>
-  <si>
-    <t>%BaseDir%\Workbench</t>
-  </si>
-  <si>
-    <t>%GlobalTemp%</t>
-  </si>
-  <si>
-    <t>%BaseDir%\Temp</t>
-  </si>
-  <si>
-    <t>%GlobalTemplates%</t>
-  </si>
-  <si>
-    <t>%Month%</t>
-  </si>
-  <si>
-    <t>%ProgramFilesDir%</t>
-  </si>
-  <si>
-    <t>C:\Program Files (x86)</t>
-  </si>
-  <si>
-    <t>%Programs64%</t>
-  </si>
-  <si>
-    <t>C:\Program Files</t>
-  </si>
-  <si>
-    <t>%SourceArch%</t>
-  </si>
-  <si>
-    <t>x64</t>
-  </si>
-  <si>
-    <t>%SourceDir%</t>
-  </si>
-  <si>
-    <t>E:\WinPE\Source\Win10x64</t>
-  </si>
-  <si>
-    <t>%SystemDrive%</t>
-  </si>
-  <si>
-    <t>#$pSystemDrive#$p</t>
-  </si>
-  <si>
-    <t>%SysType%</t>
-  </si>
-  <si>
-    <t>X64</t>
-  </si>
-  <si>
-    <t>%TargetWOW64%</t>
-  </si>
-  <si>
-    <t>x86</t>
-  </si>
-  <si>
-    <t>%TempDir%</t>
-  </si>
-  <si>
-    <t>C:\Users\Joveler\AppData\Local\Temp</t>
-  </si>
-  <si>
-    <t>%UserName%</t>
-  </si>
-  <si>
-    <t>Joveler</t>
-  </si>
-  <si>
-    <t>%UserProfile%</t>
-  </si>
-  <si>
-    <t>C:\Users\Joveler</t>
-  </si>
-  <si>
-    <t>%Version%</t>
-  </si>
-  <si>
-    <t>%WBexe%</t>
-  </si>
-  <si>
-    <t>%BaseDir%\BuilderSE.exe</t>
-  </si>
-  <si>
-    <t>%WindowsDir%</t>
-  </si>
-  <si>
-    <t>C:\WINDOWS</t>
-  </si>
-  <si>
-    <t>%WindowsSystemDir%</t>
-  </si>
-  <si>
-    <t>C:\WINDOWS\system32</t>
-  </si>
-  <si>
-    <t>%Wow64%</t>
-  </si>
-  <si>
-    <t>%Wow64Dir%</t>
-  </si>
-  <si>
-    <t>C:\WINDOWS\SysWoW64</t>
-  </si>
-  <si>
-    <t>%Year%</t>
-  </si>
-  <si>
-    <t>Test Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Support</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WB082 Test Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WB082</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exists</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Detail</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RebuildVars</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%BaseDir%\Workbench\Common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%ProcessorType%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%HostOS%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XP, W2003, WinVista</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Host OS's lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source media's lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Default Global Variables</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%ScriptFile%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%PluginFile%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;name of plugin&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foreign plugin's section not implemented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1448,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1464,27 +1472,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>22</v>
@@ -1495,7 +1503,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1503,7 +1511,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1511,7 +1519,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1519,7 +1527,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1527,7 +1535,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1535,7 +1543,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1546,11 +1554,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1561,9 +1569,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
@@ -1573,23 +1584,26 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1600,11 +1614,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>48</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1612,12 +1626,12 @@
         <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -1625,17 +1639,17 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1643,14 +1657,14 @@
         <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1658,15 +1672,15 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1675,7 +1689,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1684,7 +1698,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1693,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1702,7 +1716,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1711,7 +1725,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="1"/>
     </row>
@@ -1720,13 +1734,13 @@
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>21</v>
@@ -1740,11 +1754,11 @@
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="s">
-        <v>48</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1752,7 +1766,7 @@
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1760,7 +1774,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1768,7 +1782,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1776,7 +1790,7 @@
         <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1785,899 +1799,911 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
       <c r="D33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="4" t="s">
+      <c r="D44" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="3" t="s">
+      <c r="D45" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="3" t="s">
+      <c r="D46" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="3" t="s">
+      <c r="D47" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D48" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="F68" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D85" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F86" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>180</v>
+        <v>259</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B96" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D106" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B113" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C115" s="1">
         <v>0.7</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B116" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -2688,7 +2714,7 @@
         <v>0.8</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="2" t="s">
@@ -2697,67 +2723,67 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -2765,13 +2791,13 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C146">
         <f>COUNTA($D$2:$D$144)</f>
@@ -2780,11 +2806,11 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C147">
         <f>COUNTA($C$2:$C$144)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -2804,7 +2830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2819,370 +2845,370 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>244</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B4" s="7">
         <v>29</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B6" s="7"/>
       <c r="D6" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B11" s="7"/>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B12" s="7">
         <v>8</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B13" s="7">
         <v>8664</v>
       </c>
       <c r="D13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D16" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D19" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D20" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D22" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D23" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B24" s="7">
         <v>82</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D25" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D26" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D27" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B28" s="12" t="b">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D29" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B30" s="7">
         <v>2016</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3210,48 +3236,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>244</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E3" s="13"/>
     </row>
@@ -3259,10 +3285,10 @@
       <c r="A4" s="3"/>
       <c r="B4" s="7"/>
       <c r="C4" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E4" s="13"/>
     </row>
@@ -3271,10 +3297,10 @@
       <c r="B5" s="7"/>
       <c r="C5" s="9"/>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Collect active plugins enabled, but need some refactor NOTE: This version can pollute your volume root directory
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="263">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1021,6 +1021,10 @@
   </si>
   <si>
     <t>Encoding option added</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1028,6 +1032,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1113,7 +1120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1140,6 +1147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1456,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2800,8 +2808,8 @@
         <v>175</v>
       </c>
       <c r="C146">
-        <f>COUNTA($D$2:$D$144)</f>
-        <v>130</v>
+        <f>COUNTA($D$2:$D$144)-COUNTIF($D$2:$D$144, "Deprecated")</f>
+        <v>117</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2814,7 +2822,13 @@
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="5"/>
+      <c r="A148" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C148" s="14">
+        <f>(C147/C146)</f>
+        <v>0.10256410256410256</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B131:F139">
@@ -2831,7 +2845,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2895,9 +2909,6 @@
       <c r="B4" s="7">
         <v>29</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>240</v>
-      </c>
       <c r="D4" t="s">
         <v>119</v>
       </c>
@@ -2999,9 +3010,6 @@
       </c>
       <c r="B12" s="7">
         <v>8</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>240</v>
       </c>
       <c r="D12" t="s">
         <v>119</v>
@@ -3222,7 +3230,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3284,24 +3292,14 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D4" t="s">
-        <v>242</v>
-      </c>
+      <c r="C4" s="9"/>
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9"/>
-      <c r="D5" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>251</v>
-      </c>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>

</xml_diff>

<commit_message>
Implementing System commands (4 subcommand) +Fix circular reference infinite loop bug in varaibles
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="264">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1012,10 +1012,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PEBakery is new implementation of WinBuilder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Unicode supported</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1025,6 +1021,14 @@
   </si>
   <si>
     <t>Percentage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery's new var handling solves this problem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery is new implementation of WinBuilder Script</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1464,8 +1468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1626,7 +1630,7 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,7 +1770,7 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2336,13 +2340,16 @@
         <v>119</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="C94" s="1">
+        <v>1</v>
+      </c>
       <c r="D94" s="1" t="s">
         <v>120</v>
       </c>
@@ -2351,6 +2358,9 @@
       <c r="B95" s="3" t="s">
         <v>130</v>
       </c>
+      <c r="C95" s="1">
+        <v>1</v>
+      </c>
       <c r="D95" s="1" t="s">
         <v>120</v>
       </c>
@@ -2421,6 +2431,9 @@
       <c r="B103" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="C103" s="1">
+        <v>1</v>
+      </c>
       <c r="D103" s="1" t="s">
         <v>120</v>
       </c>
@@ -2457,7 +2470,10 @@
         <v>244</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>120</v>
+        <v>92</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
@@ -2491,6 +2507,9 @@
       <c r="B111" s="3" t="s">
         <v>125</v>
       </c>
+      <c r="C111" s="1">
+        <v>1</v>
+      </c>
       <c r="D111" s="1" t="s">
         <v>113</v>
       </c>
@@ -2809,7 +2828,7 @@
       </c>
       <c r="C146">
         <f>COUNTA($D$2:$D$144)-COUNTIF($D$2:$D$144, "Deprecated")</f>
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -2818,16 +2837,16 @@
       </c>
       <c r="C147">
         <f>COUNTA($C$2:$C$144)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C148" s="14">
         <f>(C147/C146)</f>
-        <v>0.10256410256410256</v>
+        <v>0.13793103448275862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rewrote Logger.cs, Add log functionability to Variables.cs
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="269">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,10 +139,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PERMANENT not implemented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>INI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -798,36 +794,12 @@
     <t>%Day%</t>
   </si>
   <si>
-    <t>%DistLang%</t>
-  </si>
-  <si>
-    <t>ko-KR</t>
-  </si>
-  <si>
-    <t>%DistLangHost%</t>
-  </si>
-  <si>
     <t>%FileVersion%</t>
   </si>
   <si>
     <t>82.0.0.15</t>
   </si>
   <si>
-    <t>%GlobalSupport%</t>
-  </si>
-  <si>
-    <t>%BaseDir%\Workbench</t>
-  </si>
-  <si>
-    <t>%GlobalTemp%</t>
-  </si>
-  <si>
-    <t>%BaseDir%\Temp</t>
-  </si>
-  <si>
-    <t>%GlobalTemplates%</t>
-  </si>
-  <si>
     <t>%Month%</t>
   </si>
   <si>
@@ -843,36 +815,12 @@
     <t>C:\Program Files</t>
   </si>
   <si>
-    <t>%SourceArch%</t>
-  </si>
-  <si>
-    <t>x64</t>
-  </si>
-  <si>
     <t>%SourceDir%</t>
   </si>
   <si>
     <t>E:\WinPE\Source\Win10x64</t>
   </si>
   <si>
-    <t>%SystemDrive%</t>
-  </si>
-  <si>
-    <t>#$pSystemDrive#$p</t>
-  </si>
-  <si>
-    <t>%SysType%</t>
-  </si>
-  <si>
-    <t>X64</t>
-  </si>
-  <si>
-    <t>%TargetWOW64%</t>
-  </si>
-  <si>
-    <t>x86</t>
-  </si>
-  <si>
     <t>%TempDir%</t>
   </si>
   <si>
@@ -956,79 +904,150 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>%BaseDir%\Workbench\Common</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>%HostOS%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Default Global Variables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%ScriptFile%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%PluginFile%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;name of plugin&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreign plugin's section not implemented</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INIWrite</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unicode supported</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoding option added</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery's new var handling solves this problem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery is new implementation of WinBuilder Script</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%AppMode%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wbaNormal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%Comp80%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of these values : XP, W2003, WinVista
+In PEBakery, this value is Win version number
+(Ex 10.0.14393.105)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%IsoDir%</t>
+  </si>
+  <si>
+    <t>%IsoFile%</t>
+  </si>
+  <si>
+    <t>%baseDir%\ISO\Win10PE.iso</t>
+  </si>
+  <si>
+    <t>%IsoFileName%</t>
+  </si>
+  <si>
+    <t>Win10PE.iso</t>
   </si>
   <si>
     <t>%ProcessorType%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%HostOS%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XP, W2003, WinVista</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Host OS's lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source media's lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Default Global Variables</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%ScriptFile%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>%PluginFile%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;name of plugin&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foreign plugin's section not implemented</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INIWrite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unicode supported</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Encoding option added</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percentage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery's new var handling solves this problem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery is new implementation of WinBuilder Script</t>
+  </si>
+  <si>
+    <t>%ProjectDir%</t>
+  </si>
+  <si>
+    <t>%BaseDir%\Projects\Win10PESE</t>
+  </si>
+  <si>
+    <t>%ProjectTitle%</t>
+  </si>
+  <si>
+    <t>Win10PE SE</t>
+  </si>
+  <si>
+    <t>%TargetDir%</t>
+  </si>
+  <si>
+    <t>%baseDir%\Target\Win10PESE</t>
+  </si>
+  <si>
+    <t>%Tools%</t>
+  </si>
+  <si>
+    <t>%BaseDir%\Projects\Tools</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>8664</t>
+  </si>
+  <si>
+    <t>082</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>Not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== %Temp%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%baseDir%\ISO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1124,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1152,6 +1171,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1468,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1484,27 +1512,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>22</v>
@@ -1515,7 +1543,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1523,7 +1551,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1531,7 +1559,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1539,7 +1567,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1547,7 +1575,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1555,7 +1583,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1566,11 +1594,11 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,11 +1609,11 @@
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1596,26 +1624,26 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1626,11 +1654,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1638,12 +1666,12 @@
         <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>0</v>
@@ -1651,17 +1679,17 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1">
         <v>0.8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1672,11 +1700,11 @@
         <v>0.8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1684,15 +1712,15 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -1701,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1710,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1719,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="1"/>
     </row>
@@ -1728,7 +1756,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1737,7 +1765,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="1"/>
     </row>
@@ -1746,13 +1774,13 @@
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>21</v>
@@ -1766,11 +1794,11 @@
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1778,7 +1806,7 @@
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1786,7 +1814,7 @@
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1794,7 +1822,7 @@
         <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1802,935 +1830,938 @@
         <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D85" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>116</v>
+      </c>
+      <c r="B92" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C94" s="1">
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C95" s="1">
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B96" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B113" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C115" s="1">
         <v>0.7</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B116" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0.7</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -2738,79 +2769,85 @@
         <v>28</v>
       </c>
       <c r="C136" s="1">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="2" t="s">
-        <v>29</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="C139" s="1">
+        <v>0.9</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E139" s="1"/>
+      <c r="F139" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -2818,13 +2855,13 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C146">
         <f>COUNTA($D$2:$D$144)-COUNTIF($D$2:$D$144, "Deprecated")</f>
@@ -2833,20 +2870,20 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C147">
         <f>COUNTA($C$2:$C$144)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="C148" s="14">
         <f>(C147/C146)</f>
-        <v>0.13793103448275862</v>
+        <v>0.15517241379310345</v>
       </c>
     </row>
   </sheetData>
@@ -2861,10 +2898,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2873,370 +2910,366 @@
     <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="9"/>
     <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31" style="13" customWidth="1"/>
+    <col min="5" max="5" width="43.75" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="B2" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>91</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" s="7">
-        <v>29</v>
+        <v>191</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>251</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="7"/>
+        <v>193</v>
+      </c>
+      <c r="B6" s="7">
+        <v>29</v>
+      </c>
       <c r="D6" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>250</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>240</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="B8" s="7"/>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>225</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>202</v>
+        <v>246</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="B11" s="7"/>
+        <v>249</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>250</v>
+      </c>
       <c r="D11" t="s">
-        <v>242</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="7">
-        <v>8</v>
+        <v>196</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="B13" s="7">
-        <v>8664</v>
+        <v>251</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>261</v>
       </c>
       <c r="D13" t="s">
-        <v>247</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="D24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="D25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="D26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D18" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="D27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B28" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="B29" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="D29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D20" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="D21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="D23" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="B24" s="7">
-        <v>82</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="D24" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="D25" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="D26" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="D27" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B28" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="D29" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B30" s="7">
-        <v>2016</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>240</v>
+      <c r="B30" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="D30" t="s">
-        <v>119</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3263,48 +3296,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="E3" s="13"/>
     </row>

</xml_diff>

<commit_message>
Implemented system subcommands (7 cmds), ShellExecute seires
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="274">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1048,6 +1048,26 @@
   </si>
   <si>
     <t>Need test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShellExecuteEx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShellExecuteDelete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run's #1 not supported, not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run's #1 not supported, not used in WinPESE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1494,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1507,7 +1527,7 @@
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1808,6 +1828,9 @@
       <c r="D28" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F28" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
@@ -1816,6 +1839,9 @@
       <c r="D29" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F29" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
@@ -1824,6 +1850,9 @@
       <c r="D30" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F30" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
@@ -1832,6 +1861,9 @@
       <c r="D31" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="F31" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
@@ -2408,6 +2440,9 @@
       <c r="B97" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="C97" s="1">
+        <v>1</v>
+      </c>
       <c r="D97" s="1" t="s">
         <v>119</v>
       </c>
@@ -2416,6 +2451,9 @@
       <c r="B98" s="3" t="s">
         <v>131</v>
       </c>
+      <c r="C98" s="1">
+        <v>1</v>
+      </c>
       <c r="D98" s="1" t="s">
         <v>119</v>
       </c>
@@ -2424,6 +2462,9 @@
       <c r="B99" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="C99" s="1">
+        <v>1</v>
+      </c>
       <c r="D99" s="1" t="s">
         <v>119</v>
       </c>
@@ -2443,6 +2484,9 @@
       <c r="B101" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="C101" s="1">
+        <v>1</v>
+      </c>
       <c r="D101" s="1" t="s">
         <v>119</v>
       </c>
@@ -2470,22 +2514,37 @@
       <c r="B104" s="3" t="s">
         <v>137</v>
       </c>
+      <c r="C104" s="1">
+        <v>1</v>
+      </c>
       <c r="D104" s="1" t="s">
-        <v>119</v>
+        <v>271</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="3" t="s">
         <v>138</v>
       </c>
+      <c r="C105" s="1">
+        <v>1</v>
+      </c>
       <c r="D105" s="1" t="s">
-        <v>119</v>
+        <v>271</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="C106" s="1">
+        <v>1</v>
+      </c>
       <c r="D106" t="s">
         <v>109</v>
       </c>
@@ -2557,62 +2616,71 @@
       <c r="B113" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="C113" s="1">
+        <v>1</v>
+      </c>
       <c r="D113" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>165</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>142</v>
+      <c r="B114" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C114" s="1">
+        <v>1</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>143</v>
+        <v>270</v>
       </c>
       <c r="C115" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>233</v>
+        <v>52</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B116" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C116" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>112</v>
+      <c r="A116" t="s">
+        <v>165</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0.7</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="F117" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>182</v>
+        <v>144</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0.7</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>112</v>
@@ -2620,18 +2688,15 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>146</v>
+        <v>182</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>112</v>
@@ -2639,18 +2704,18 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>112</v>
@@ -2658,45 +2723,45 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="F124" s="2" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>118</v>
@@ -2707,7 +2772,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>112</v>
@@ -2715,15 +2780,18 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>112</v>
@@ -2731,159 +2799,175 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>52</v>
+        <v>118</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>167</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>166</v>
+      <c r="B135" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C136" s="1">
-        <v>0.9</v>
+        <v>73</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E136" s="1"/>
-      <c r="F136" s="2" t="s">
-        <v>268</v>
-      </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B137" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>164</v>
+      <c r="A137" t="s">
+        <v>167</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0.9</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E138" s="1"/>
       <c r="F138" s="2" t="s">
-        <v>164</v>
+        <v>268</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C139" s="1">
-        <v>0.9</v>
+        <v>50</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E139" s="1"/>
       <c r="F139" s="2" t="s">
-        <v>268</v>
+        <v>164</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E140" s="1"/>
+      <c r="F140" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="C141" s="1">
+        <v>0.9</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E141" s="1"/>
+      <c r="F141" s="2" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E143" s="1"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B144" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B145" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D144" s="1"/>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="6" t="s">
+      <c r="D145" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D146" s="1"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="C145" s="3"/>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="5" t="s">
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C146">
-        <f>COUNTA($D$2:$D$144)-COUNTIF($D$2:$D$144, "Deprecated")</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="5" t="s">
+      <c r="C148">
+        <f>COUNTA($D$2:$D$146)-COUNTIF($D$2:$D$146, "Deprecated")</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C147">
-        <f>COUNTA($C$2:$C$144)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="5" t="s">
+      <c r="C149">
+        <f>COUNTA($C$2:$C$146)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C148" s="14">
-        <f>(C147/C146)</f>
-        <v>0.15517241379310345</v>
+      <c r="C150" s="14">
+        <f>(C149/C148)</f>
+        <v>0.23728813559322035</v>
       </c>
     </row>
   </sheetData>
@@ -2900,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implemented If,ExistFile / If,ExistDir command
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="283">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -599,18 +599,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Exec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>If,Exist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>If,NotExist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>If,Begin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -735,14 +727,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>==If,Not,Equal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>==If,Not,Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>== StrFormat,DirPath</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -921,10 +905,6 @@
   </si>
   <si>
     <t>&lt;name of plugin&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foreign plugin's section not implemented</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1068,6 +1048,62 @@
   </si>
   <si>
     <t>Run's #1 not supported, not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistDir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistRegSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistRegKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistVar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExistFile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExistDir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExistSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExistRegSection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExistRegKey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotExistVar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Supported for compability. Will be deprecated in favor of If,Not</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1514,10 +1550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1527,7 +1563,7 @@
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -1535,7 +1571,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>20</v>
@@ -1544,7 +1580,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>36</v>
@@ -1633,7 +1669,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1648,7 +1684,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1663,7 +1699,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1674,11 +1710,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1818,7 +1854,7 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1829,7 +1865,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1840,7 +1876,7 @@
         <v>52</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1851,7 +1887,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1862,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1882,12 +1918,12 @@
         <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -1896,7 +1932,7 @@
         <v>52</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2100,35 +2136,35 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2209,7 +2245,7 @@
         <v>52</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
@@ -2332,26 +2368,26 @@
         <v>112</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>141</v>
@@ -2381,7 +2417,7 @@
         <v>112</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2400,7 +2436,7 @@
         <v>118</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2518,10 +2554,10 @@
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
@@ -2532,10 +2568,10 @@
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
@@ -2549,18 +2585,18 @@
         <v>109</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
@@ -2625,7 +2661,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -2636,7 +2672,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -2647,7 +2683,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>142</v>
@@ -2658,29 +2694,26 @@
         <v>143</v>
       </c>
       <c r="C117" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>233</v>
-      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>144</v>
+        <v>275</v>
       </c>
       <c r="C118" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>112</v>
@@ -2688,7 +2721,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>119</v>
@@ -2696,278 +2729,388 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>145</v>
+        <v>269</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>146</v>
+        <v>270</v>
+      </c>
+      <c r="C122" s="1">
+        <v>1</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>179</v>
+        <v>41</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>148</v>
+        <v>271</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>149</v>
+        <v>272</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>178</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>150</v>
+        <v>273</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>151</v>
+        <v>274</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>152</v>
+        <v>276</v>
+      </c>
+      <c r="C127" s="1">
+        <v>1</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>141</v>
+        <v>282</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>154</v>
+        <v>277</v>
+      </c>
+      <c r="C128" s="1">
+        <v>1</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>155</v>
+        <v>278</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>156</v>
+        <v>279</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>157</v>
+        <v>280</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>158</v>
+        <v>281</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="D134" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B135" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B136" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B137" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D137" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F134" s="2" t="s">
+      <c r="F137" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B135" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B136" s="3" t="s">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B138" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B139" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B140" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B141" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C141" s="1">
+        <v>1</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B142" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B143" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B144" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B145" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B146" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>167</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B138" s="3" t="s">
+      <c r="D146" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>165</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B148" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C138" s="1">
+      <c r="C148" s="1">
         <v>0.9</v>
       </c>
-      <c r="D138" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E138" s="1"/>
-      <c r="F138" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B139" s="3" t="s">
+      <c r="D148" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E148" s="1"/>
+      <c r="F148" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B149" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D139" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F139" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B140" s="3" t="s">
+      <c r="D149" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B150" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B141" s="3" t="s">
+      <c r="D150" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B151" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C141" s="1">
+      <c r="C151" s="1">
         <v>0.9</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E141" s="1"/>
-      <c r="F141" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B142" s="3" t="s">
+      <c r="D151" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E151" s="1"/>
+      <c r="F151" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B152" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E142" s="1"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B143" s="3" t="s">
+      <c r="D152" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E152" s="1"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B153" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D143" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E143" s="1"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B144" s="3" t="s">
+      <c r="D153" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E153" s="1"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B154" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B145" s="3" t="s">
+      <c r="D154" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B155" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D145" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D146" s="1"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="C147" s="3"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C148">
-        <f>COUNTA($D$2:$D$146)-COUNTIF($D$2:$D$146, "Deprecated")</f>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C149">
-        <f>COUNTA($C$2:$C$146)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C150" s="14">
-        <f>(C149/C148)</f>
-        <v>0.23728813559322035</v>
+      <c r="D155" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C158">
+        <f>COUNTA($D$2:$D$156)-COUNTIF($D$2:$D$156, "Deprecated")</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C159">
+        <f>COUNTA($C$2:$C$156)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C160" s="14">
+        <f>(C159/C158)</f>
+        <v>0.2578125</v>
       </c>
     </row>
   </sheetData>
@@ -2999,69 +3142,69 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D2" t="s">
         <v>91</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D5" t="s">
         <v>91</v>
@@ -3069,7 +3212,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B6" s="7">
         <v>29</v>
@@ -3080,69 +3223,69 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B8" s="7"/>
       <c r="D8" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D9" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -3150,10 +3293,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D13" t="s">
         <v>91</v>
@@ -3161,189 +3304,189 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D14" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D20" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D21" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D22" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D23" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D24" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D26" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D27" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D28" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D29" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D30" t="s">
         <v>91</v>
@@ -3380,48 +3523,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>224</v>
-      </c>
       <c r="E1" s="8" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E3" s="13"/>
     </row>

</xml_diff>

<commit_message>
Fixed bug occurs if OnBuildExit, OnPluginExit is used with Run
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="282">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -596,10 +596,6 @@
   </si>
   <si>
     <t>Run</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Exist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1552,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1571,7 +1567,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>20</v>
@@ -1580,7 +1576,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>36</v>
@@ -1669,7 +1665,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1684,7 +1680,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1699,7 +1695,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1710,11 +1706,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1854,7 +1850,7 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1865,7 +1861,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1876,7 +1872,7 @@
         <v>52</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1887,7 +1883,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1898,7 +1894,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1918,12 +1914,12 @@
         <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -1932,7 +1928,7 @@
         <v>52</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2136,35 +2132,35 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2245,7 +2241,7 @@
         <v>52</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
@@ -2368,26 +2364,26 @@
         <v>112</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>141</v>
@@ -2417,7 +2413,7 @@
         <v>112</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2436,7 +2432,7 @@
         <v>118</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2554,10 +2550,10 @@
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
@@ -2568,10 +2564,10 @@
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
@@ -2585,18 +2581,18 @@
         <v>109</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
@@ -2661,7 +2657,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -2672,7 +2668,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -2683,7 +2679,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>142</v>
@@ -2702,7 +2698,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -2713,7 +2709,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>112</v>
@@ -2721,7 +2717,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>119</v>
@@ -2729,7 +2725,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C121" s="1">
         <v>1</v>
@@ -2740,7 +2736,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -2751,7 +2747,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+      <c r="C123" s="1">
+        <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>41</v>
@@ -2759,7 +2758,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>41</v>
@@ -2767,7 +2766,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>41</v>
@@ -2775,7 +2774,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>41</v>
@@ -2783,7 +2782,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -2792,12 +2791,12 @@
         <v>41</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -2806,56 +2805,59 @@
         <v>41</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
+      </c>
+      <c r="C129" s="1">
+        <v>1</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>112</v>
@@ -2863,18 +2865,18 @@
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>112</v>
@@ -2882,7 +2884,7 @@
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>112</v>
@@ -2890,7 +2892,7 @@
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>118</v>
@@ -2901,7 +2903,7 @@
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>118</v>
@@ -2912,7 +2914,7 @@
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>112</v>
@@ -2920,7 +2922,7 @@
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>118</v>
@@ -2931,7 +2933,7 @@
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C141" s="1">
         <v>1</v>
@@ -2942,7 +2944,7 @@
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>112</v>
@@ -2950,7 +2952,7 @@
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>112</v>
@@ -2958,7 +2960,7 @@
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>118</v>
@@ -2969,7 +2971,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B145" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>52</v>
@@ -2985,10 +2987,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3003,7 +3005,7 @@
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3014,7 +3016,7 @@
         <v>52</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3025,7 +3027,7 @@
         <v>52</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3040,7 +3042,7 @@
       </c>
       <c r="E151" s="1"/>
       <c r="F151" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3082,13 +3084,13 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C158">
         <f>COUNTA($D$2:$D$156)-COUNTIF($D$2:$D$156, "Deprecated")</f>
@@ -3097,20 +3099,20 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C159">
         <f>COUNTA($C$2:$C$156)</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C160" s="14">
         <f>(C159/C158)</f>
-        <v>0.2578125</v>
+        <v>0.2734375</v>
       </c>
     </row>
   </sheetData>
@@ -3142,69 +3144,69 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="D2" t="s">
         <v>91</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>188</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="D5" t="s">
         <v>91</v>
@@ -3212,7 +3214,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" s="7">
         <v>29</v>
@@ -3223,69 +3225,69 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8" s="7"/>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>245</v>
-      </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -3293,10 +3295,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D13" t="s">
         <v>91</v>
@@ -3304,189 +3306,189 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="D15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>248</v>
-      </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>250</v>
-      </c>
       <c r="D17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>198</v>
-      </c>
       <c r="D18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>200</v>
-      </c>
       <c r="D20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>254</v>
-      </c>
       <c r="D21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="D22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="D23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="D25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>209</v>
-      </c>
       <c r="D26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="D27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="D29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D30" t="s">
         <v>91</v>
@@ -3523,48 +3525,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>217</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>228</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E3" s="13"/>
     </row>

</xml_diff>

<commit_message>
Implemented If compare (Equal, Smaller, Bigger)
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="283">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -596,10 +596,6 @@
   </si>
   <si>
     <t>Run</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Begin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1100,6 +1096,14 @@
   </si>
   <si>
     <t>Supported for compability. Will be deprecated in favor of If,Not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Begin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Does not work 100% same with WB, need check</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1548,8 +1552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1567,7 +1571,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>20</v>
@@ -1576,7 +1580,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>36</v>
@@ -1665,7 +1669,7 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1680,7 +1684,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1695,7 +1699,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1706,11 +1710,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1850,7 +1854,7 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1861,7 +1865,7 @@
         <v>52</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1872,7 +1876,7 @@
         <v>52</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1883,7 +1887,7 @@
         <v>52</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1894,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1914,12 +1918,12 @@
         <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -1928,7 +1932,7 @@
         <v>52</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2132,35 +2136,35 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2241,7 +2245,7 @@
         <v>52</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
@@ -2364,26 +2368,26 @@
         <v>112</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>141</v>
@@ -2413,7 +2417,7 @@
         <v>112</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
@@ -2432,7 +2436,7 @@
         <v>118</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
@@ -2550,10 +2554,10 @@
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
@@ -2564,10 +2568,10 @@
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
@@ -2581,18 +2585,18 @@
         <v>109</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
@@ -2657,7 +2661,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -2668,7 +2672,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -2679,7 +2683,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>142</v>
@@ -2698,7 +2702,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -2709,7 +2713,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>144</v>
+        <v>281</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>112</v>
@@ -2717,7 +2721,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>119</v>
@@ -2725,7 +2729,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C121" s="1">
         <v>1</v>
@@ -2736,7 +2740,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -2747,7 +2751,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -2758,7 +2762,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>41</v>
@@ -2766,15 +2773,24 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0.8</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="F125" s="2" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="C126" s="1">
+        <v>1</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>41</v>
@@ -2782,7 +2798,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -2791,12 +2807,12 @@
         <v>41</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -2805,12 +2821,12 @@
         <v>41</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -2819,45 +2835,57 @@
         <v>41</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0.8</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
+      </c>
+      <c r="C132" s="1">
+        <v>1</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
+      </c>
+      <c r="C133" s="1">
+        <v>1</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>112</v>
@@ -2865,18 +2893,21 @@
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>112</v>
@@ -2884,7 +2915,7 @@
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>112</v>
@@ -2892,7 +2923,7 @@
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>118</v>
@@ -2903,7 +2934,7 @@
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>118</v>
@@ -2914,7 +2945,7 @@
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>112</v>
@@ -2922,7 +2953,7 @@
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>118</v>
@@ -2933,7 +2964,7 @@
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C141" s="1">
         <v>1</v>
@@ -2944,7 +2975,7 @@
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>112</v>
@@ -2952,7 +2983,7 @@
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>112</v>
@@ -2960,7 +2991,7 @@
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>118</v>
@@ -2971,7 +3002,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B145" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>52</v>
@@ -2987,10 +3018,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
@@ -3005,7 +3036,7 @@
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
@@ -3016,7 +3047,7 @@
         <v>52</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
@@ -3027,7 +3058,7 @@
         <v>52</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
@@ -3042,7 +3073,7 @@
       </c>
       <c r="E151" s="1"/>
       <c r="F151" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3084,13 +3115,13 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C158">
         <f>COUNTA($D$2:$D$156)-COUNTIF($D$2:$D$156, "Deprecated")</f>
@@ -3099,20 +3130,20 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C159">
         <f>COUNTA($C$2:$C$156)</f>
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C160" s="14">
         <f>(C159/C158)</f>
-        <v>0.2734375</v>
+        <v>0.3359375</v>
       </c>
     </row>
   </sheetData>
@@ -3144,69 +3175,69 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="D2" t="s">
         <v>91</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>185</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>187</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="D5" t="s">
         <v>91</v>
@@ -3214,7 +3245,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6" s="7">
         <v>29</v>
@@ -3225,69 +3256,69 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>190</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" s="7"/>
       <c r="D8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>242</v>
-      </c>
       <c r="D10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" t="s">
         <v>91</v>
@@ -3295,10 +3326,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D13" t="s">
         <v>91</v>
@@ -3306,189 +3337,189 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>193</v>
-      </c>
       <c r="D14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>247</v>
-      </c>
       <c r="D16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>249</v>
-      </c>
       <c r="D17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>197</v>
-      </c>
       <c r="D18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>251</v>
-      </c>
       <c r="D19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>199</v>
-      </c>
       <c r="D20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>253</v>
-      </c>
       <c r="D21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>201</v>
-      </c>
       <c r="D22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>203</v>
-      </c>
       <c r="D23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="D25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="D26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="D27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>213</v>
-      </c>
       <c r="D29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D30" t="s">
         <v>91</v>
@@ -3525,48 +3556,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>216</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>227</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E3" s="13"/>
     </row>

</xml_diff>

<commit_message>
Verbose logging to set, branch experiment I HATE BRANCH COMMAND! (If, Else, Begin, End) Should make compiler to convert script to goto-style commands!
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="292">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1019,10 +1019,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Need test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ShellExecuteEx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1103,7 +1099,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Does not work 100% same with WB, need check</t>
+    <t>If,SmallerEqual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,BiggerEqual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias : &lt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias : &lt;=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias : &gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias : &gt;=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias : ==</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alias : !=, Same with If,Not,%Variable%,Equal,Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Does not work 100% same with WB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1550,10 +1586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F160"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1563,7 +1599,7 @@
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60.75" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2554,10 +2590,10 @@
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
@@ -2568,10 +2604,10 @@
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
@@ -2661,7 +2697,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -2672,7 +2708,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -2702,7 +2738,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -2713,7 +2749,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>112</v>
@@ -2729,7 +2765,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C121" s="1">
         <v>1</v>
@@ -2740,7 +2776,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C122" s="1">
         <v>1</v>
@@ -2751,7 +2787,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
@@ -2762,7 +2798,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -2773,7 +2809,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C125" s="1">
         <v>0.8</v>
@@ -2782,12 +2818,12 @@
         <v>41</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -2798,7 +2834,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -2807,12 +2843,12 @@
         <v>41</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -2821,12 +2857,12 @@
         <v>41</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C129" s="1">
         <v>1</v>
@@ -2835,12 +2871,12 @@
         <v>41</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -2849,12 +2885,12 @@
         <v>41</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C131" s="1">
         <v>0.8</v>
@@ -2863,12 +2899,12 @@
         <v>41</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -2877,7 +2913,7 @@
         <v>41</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
@@ -2890,6 +2926,9 @@
       <c r="D133" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="F133" s="2" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
@@ -2902,72 +2941,87 @@
         <v>112</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
         <v>146</v>
       </c>
+      <c r="C135" s="1">
+        <v>1</v>
+      </c>
       <c r="D135" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>147</v>
+        <v>281</v>
+      </c>
+      <c r="C136" s="1">
+        <v>1</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>112</v>
+        <v>283</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
+      </c>
+      <c r="C137" s="1">
+        <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>141</v>
+        <v>287</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>150</v>
+        <v>282</v>
+      </c>
+      <c r="C138" s="1">
+        <v>1</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>118</v>
+        <v>284</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>141</v>
+        <v>288</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C141" s="1">
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>112</v>
@@ -2975,15 +3029,21 @@
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>112</v>
+        <v>118</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="C143" s="1">
+        <v>1</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>112</v>
@@ -2991,103 +3051,95 @@
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B145" s="3" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B146" s="3" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>52</v>
+        <v>118</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>163</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>162</v>
+      <c r="B147" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B148" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C148" s="1">
-        <v>0.9</v>
+        <v>73</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E148" s="1"/>
-      <c r="F148" s="2" t="s">
-        <v>261</v>
-      </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B149" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F149" s="2" t="s">
-        <v>160</v>
+      <c r="A149" t="s">
+        <v>163</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B150" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
+      </c>
+      <c r="C150" s="1">
+        <v>1</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F150" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B151" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C151" s="1">
-        <v>0.9</v>
+        <v>50</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E151" s="1"/>
       <c r="F151" s="2" t="s">
-        <v>261</v>
+        <v>160</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B152" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E152" s="1"/>
+      <c r="F152" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B153" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="C153" s="1">
+        <v>1</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>52</v>
@@ -3096,54 +3148,72 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B154" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B155" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E155" s="1"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B156" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B157" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="6" t="s">
+      <c r="D157" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C157" s="3"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C158">
-        <f>COUNTA($D$2:$D$156)-COUNTIF($D$2:$D$156, "Deprecated")</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C159">
-        <f>COUNTA($C$2:$C$156)</f>
-        <v>43</v>
-      </c>
+      <c r="C159" s="3"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C160">
+        <f>COUNTA($D$2:$D$158)-COUNTIF($D$2:$D$158, "Deprecated")</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C161">
+        <f>COUNTA($C$2:$C$158)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C160" s="14">
-        <f>(C159/C158)</f>
-        <v>0.3359375</v>
+      <c r="C162" s="14">
+        <f>(C161/C160)</f>
+        <v>0.35877862595419846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Middle save while writing compiler
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="298">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -292,10 +292,6 @@
   </si>
   <si>
     <t>Echo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineNetwork.cs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1140,6 +1136,34 @@
   </si>
   <si>
     <t>Does not work 100% same with WB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jump</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primitive opcode, only appear after compiled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compiled to Jump</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1150,7 +1174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1198,14 +1222,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1235,14 +1251,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1271,6 +1285,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1586,15 +1603,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F162"/>
+  <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D141" sqref="D141"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
@@ -1602,28 +1619,28 @@
     <col min="6" max="6" width="60.75" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1705,10 +1722,13 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1720,7 +1740,7 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1735,7 +1755,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1746,11 +1766,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1762,81 +1782,76 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
       <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.8</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.8</v>
+        <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2" t="s">
-        <v>48</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
+      <c r="A18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.8</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="1"/>
+      <c r="F19" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.8</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="1"/>
+      <c r="F20" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>41</v>
@@ -1845,7 +1860,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>41</v>
@@ -1854,7 +1869,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>41</v>
@@ -1863,7 +1878,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>41</v>
@@ -1871,84 +1886,80 @@
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="2" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>229</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>229</v>
+      <c r="A29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="1"/>
+      <c r="B32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>52</v>
@@ -1959,10 +1970,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>52</v>
@@ -1972,32 +1980,42 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="B35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>33</v>
+        <v>226</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>52</v>
@@ -2005,24 +2023,23 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" s="1"/>
+      <c r="B40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>52</v>
@@ -2030,14 +2047,14 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="A43" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -2099,8 +2116,8 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>76</v>
+      <c r="A51" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>65</v>
@@ -2124,7 +2141,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>52</v>
@@ -2132,7 +2149,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>52</v>
@@ -2140,7 +2157,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>52</v>
@@ -2148,7 +2165,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>52</v>
@@ -2156,7 +2173,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>52</v>
@@ -2164,7 +2181,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>52</v>
@@ -2172,48 +2189,48 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="A63" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>52</v>
@@ -2221,7 +2238,7 @@
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>52</v>
@@ -2229,7 +2246,7 @@
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>52</v>
@@ -2237,29 +2254,29 @@
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>52</v>
@@ -2267,7 +2284,7 @@
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>52</v>
@@ -2275,26 +2292,26 @@
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>52</v>
@@ -2302,7 +2319,7 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>52</v>
@@ -2310,7 +2327,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>52</v>
@@ -2318,7 +2335,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>52</v>
@@ -2326,7 +2343,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>52</v>
@@ -2334,7 +2351,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>52</v>
@@ -2342,7 +2359,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>52</v>
@@ -2350,7 +2367,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>52</v>
@@ -2358,7 +2375,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>52</v>
@@ -2366,7 +2383,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>52</v>
@@ -2374,7 +2391,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>52</v>
@@ -2382,7 +2399,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>52</v>
@@ -2390,303 +2407,303 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="B92" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C94" s="1">
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C95" s="1">
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B96" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C98" s="1">
         <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C99" s="1">
         <v>1</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C101" s="1">
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C106" s="1">
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B113" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
@@ -2697,7 +2714,7 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
@@ -2708,7 +2725,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C115" s="1">
         <v>1</v>
@@ -2718,27 +2735,27 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>161</v>
+      <c r="A116" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -2749,81 +2766,86 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>280</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="C119" s="1"/>
       <c r="D119" s="1" t="s">
-        <v>112</v>
+        <v>294</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>176</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="C120" s="1"/>
       <c r="D120" s="1" t="s">
-        <v>119</v>
+        <v>41</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="C121" s="1">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B122" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C122" s="1">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C123" s="1">
-        <v>1</v>
+        <v>279</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>41</v>
+        <v>111</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C124" s="1">
-        <v>1</v>
+        <v>175</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>41</v>
+        <v>118</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C125" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F125" s="2" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -2834,7 +2856,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -2842,13 +2864,10 @@
       <c r="D127" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F127" s="2" t="s">
-        <v>279</v>
-      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -2856,27 +2875,24 @@
       <c r="D128" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F128" s="2" t="s">
-        <v>279</v>
-      </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C129" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -2884,27 +2900,24 @@
       <c r="D130" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F130" s="2" t="s">
-        <v>279</v>
-      </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C131" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -2913,251 +2926,273 @@
         <v>41</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>144</v>
+        <v>274</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>145</v>
+        <v>275</v>
       </c>
       <c r="C134" s="1">
         <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
       <c r="C135" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C136" s="1">
         <v>1</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>283</v>
+        <v>41</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C137" s="1">
         <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>282</v>
+        <v>144</v>
       </c>
       <c r="C138" s="1">
         <v>1</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>284</v>
+        <v>111</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="C139" s="1">
+        <v>1</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>141</v>
+        <v>284</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>150</v>
+        <v>280</v>
+      </c>
+      <c r="C140" s="1">
+        <v>1</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>41</v>
+        <v>282</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
+      </c>
+      <c r="C141" s="1">
+        <v>1</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>152</v>
+        <v>281</v>
+      </c>
+      <c r="C142" s="1">
+        <v>1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>118</v>
+        <v>283</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>141</v>
+        <v>287</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C143" s="1">
-        <v>1</v>
+        <v>147</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B145" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B146" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B147" s="3" t="s">
-        <v>177</v>
+        <v>152</v>
+      </c>
+      <c r="C147" s="1">
+        <v>1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B148" s="3" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>163</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>162</v>
+      <c r="B149" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B150" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C150" s="1">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E150" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B151" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>160</v>
+      <c r="A151" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B152" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
+      </c>
+      <c r="C152" s="1">
+        <v>1</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F152" s="2" t="s">
-        <v>160</v>
-      </c>
+      <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B153" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C153" s="1">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E153" s="1"/>
+      <c r="F153" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B154" s="3" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E154" s="1"/>
+      <c r="F154" s="2" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B155" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="C155" s="1">
+        <v>1</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>52</v>
@@ -3166,54 +3201,72 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B156" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B157" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E157" s="1"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D158" s="1"/>
+      <c r="B158" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C159" s="3"/>
+      <c r="B159" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C160">
-        <f>COUNTA($D$2:$D$158)-COUNTIF($D$2:$D$158, "Deprecated")</f>
-        <v>131</v>
-      </c>
+      <c r="D160" s="1"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="5" t="s">
+      <c r="A161" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C161">
-        <f>COUNTA($C$2:$C$158)</f>
+      <c r="C161" s="3"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C162">
+        <f>COUNTA($D$2:$D$160)-COUNTIF($D$2:$D$160, "Deprecated")</f>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C163">
+        <f>COUNTA($C$2:$C$160)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C162" s="14">
-        <f>(C161/C160)</f>
-        <v>0.35877862595419846</v>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C164" s="12">
+        <f>(C163/C162)</f>
+        <v>0.35606060606060608</v>
       </c>
     </row>
   </sheetData>
@@ -3238,368 +3291,368 @@
   <cols>
     <col min="1" max="1" width="24.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="9"/>
+    <col min="3" max="3" width="9" style="7"/>
     <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.75" style="16" customWidth="1"/>
+    <col min="5" max="5" width="43.75" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>235</v>
-      </c>
       <c r="D2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>258</v>
+        <v>90</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>217</v>
+      <c r="C3" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="D3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>217</v>
+      <c r="C4" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>237</v>
-      </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="7">
+        <v>186</v>
+      </c>
+      <c r="B6" s="5">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>217</v>
+      <c r="C7" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="D7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B8" s="7"/>
+        <v>221</v>
+      </c>
+      <c r="B8" s="5"/>
       <c r="D8" t="s">
-        <v>219</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>238</v>
+        <v>218</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>260</v>
+        <v>238</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>253</v>
+        <v>189</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>254</v>
+        <v>243</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>192</v>
-      </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>194</v>
-      </c>
       <c r="D15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>246</v>
-      </c>
       <c r="D16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>248</v>
-      </c>
       <c r="D17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="D18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>250</v>
-      </c>
       <c r="D19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>198</v>
-      </c>
       <c r="D20" t="s">
-        <v>219</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>259</v>
+        <v>218</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>252</v>
-      </c>
       <c r="D21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>200</v>
-      </c>
       <c r="D22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="D23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>255</v>
+        <v>202</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>254</v>
       </c>
       <c r="D24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="D25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>207</v>
-      </c>
       <c r="D26" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>209</v>
-      </c>
       <c r="D27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>256</v>
+        <v>209</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>212</v>
-      </c>
       <c r="D29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>257</v>
+        <v>212</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>256</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="7"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="7"/>
+      <c r="B32" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3625,213 +3678,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>220</v>
+      <c r="D1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>217</v>
+        <v>223</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E2" s="13"/>
+        <v>218</v>
+      </c>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>217</v>
+      <c r="C3" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="D3" t="s">
-        <v>219</v>
-      </c>
-      <c r="E3" s="13"/>
+        <v>218</v>
+      </c>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="9"/>
-      <c r="E4" s="13"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="E5" s="13"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="E6" s="13"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="9"/>
-      <c r="E7" s="13"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="9"/>
-      <c r="E8" s="13"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="9"/>
-      <c r="E9" s="13"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="9"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="9"/>
-      <c r="E11" s="13"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="9"/>
-      <c r="E12" s="13"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="9"/>
-      <c r="E13" s="13"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="7"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="9"/>
-      <c r="E14" s="13"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="9"/>
-      <c r="E15" s="13"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="E15" s="11"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="9"/>
-      <c r="E16" s="13"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="7"/>
+      <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="E17" s="13"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="9"/>
-      <c r="E18" s="13"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
-      <c r="E19" s="13"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7"/>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
-      <c r="E20" s="13"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-      <c r="E21" s="13"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7"/>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="9"/>
-      <c r="E22" s="13"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="7"/>
+      <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="9"/>
-      <c r="E23" s="13"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="9"/>
-      <c r="E24" s="13"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="7"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="9"/>
-      <c r="E25" s="13"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="11"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="9"/>
-      <c r="E26" s="13"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="7"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="9"/>
-      <c r="E27" s="13"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="7"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="9"/>
-      <c r="E28" s="13"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="7"/>
+      <c r="E28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="9"/>
-      <c r="E29" s="13"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="7"/>
+      <c r="E29" s="11"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="9"/>
-      <c r="E30" s="13"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="7"/>
+      <c r="E30" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
BugFix, LogInfo[] to List<LogInfo>, and lot more
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="296">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -403,7 +403,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>StrFormat,DirPath</t>
+    <t>StrFormat,Inc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Dec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Mult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Div</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat.Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Len</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,LTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,RTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,CTrim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,NTrim</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -411,47 +451,223 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>StrFormat,Inc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Dec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Mult</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Div</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Left</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat.Right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Len</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,LTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,RTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,CTrim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,NTrim</t>
+    <t>StrFormat,Pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,SubStr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,ShortPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,LongPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrFormat,Split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineSystem.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exist</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,GetEnv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,Cursor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,Log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RefreshInterface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,SaveLog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,SplitParameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RescanScript</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,RegRedirect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,Comp80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,ErrorOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,FileRedirect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,GetFreeDrive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,GetFreeSpace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,HasUAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,IsAdmin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,IsTerminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery can work across with UAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,OnBuildExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,OnScriptExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>System,OnPluginExit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEBakery is .Net Application, works without WOW64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not used in WinPESE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Branch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Equal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,NotEqual</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Smaller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Bigger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,EqualX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Ping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Online</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,License</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Not</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,Question</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistMacro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If,ExistRegMulti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extended</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>== FIleRename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Commands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will be deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineBranch.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BakeryEngineControl.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieve,SHA1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -459,234 +675,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>StrFormat,Pos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,SubStr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,ShortPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,LongPath</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StrFormat,Split</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineSystem.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exist</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,GetEnv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,Cursor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,Log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RefreshInterface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,SaveLog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,SplitParameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RescanScript</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,RegRedirect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,Comp80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,ErrorOff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,FileRedirect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,GetFreeDrive</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,GetFreeSpace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,HasUAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,IsAdmin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,IsTerminal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery can work across with UAC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,OnBuildExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,OnScriptExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System,OnPluginExit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PEBakery is .Net Application, works without WOW64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Not used in WinPESE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Branch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Run</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Equal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,NotEqual</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Smaller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Bigger</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,EqualX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Ping</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Online</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,License</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Not</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,Question</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,ExistMacro</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If,ExistRegMulti</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Extended</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>== FIleRename</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Commands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Will be deprecated</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineBranch.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Control</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BakeryEngineControl.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Retrieve,SHA1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>New</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Retrieve,SHA256</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -897,10 +889,6 @@
   </si>
   <si>
     <t>INIWrite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1147,23 +1135,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Jump</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Primitive opcode, only appear after compiled</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compiled to Jump</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>If</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compiled to IfCompact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compiled to ElseCompact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compiled to Tree Data Structre</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IfCompact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ElseCompact</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1605,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1624,7 +1616,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>20</v>
@@ -1633,7 +1625,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>36</v>
@@ -1721,13 +1713,10 @@
         <v>41</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="2" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -1739,9 +1728,6 @@
         <v>41</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="2" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
@@ -1755,7 +1741,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1766,11 +1752,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1800,7 +1786,7 @@
         <v>61</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1932,7 +1918,7 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1943,7 +1929,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1954,7 +1940,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1965,7 +1951,7 @@
         <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1976,7 +1962,7 @@
         <v>52</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1995,22 +1981,16 @@
       <c r="D36" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>227</v>
-      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C37" s="1">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2189,35 +2169,35 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -2298,20 +2278,20 @@
         <v>52</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>52</v>
@@ -2319,7 +2299,7 @@
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>52</v>
@@ -2327,7 +2307,7 @@
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>52</v>
@@ -2335,7 +2315,7 @@
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>52</v>
@@ -2343,7 +2323,7 @@
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>52</v>
@@ -2351,7 +2331,7 @@
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>52</v>
@@ -2359,7 +2339,7 @@
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>52</v>
@@ -2367,7 +2347,7 @@
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>52</v>
@@ -2375,7 +2355,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>52</v>
@@ -2383,7 +2363,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>52</v>
@@ -2391,7 +2371,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>52</v>
@@ -2399,311 +2379,314 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>52</v>
+        <v>108</v>
+      </c>
+      <c r="D84" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D85" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="F86" s="2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>179</v>
+        <v>110</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
+      <c r="B92" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>116</v>
+      <c r="F92" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
-        <v>127</v>
+        <v>118</v>
+      </c>
+      <c r="C93" s="1">
+        <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>232</v>
+        <v>116</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C94" s="1">
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C95" s="1">
-        <v>1</v>
+        <v>127</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B96" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
+      </c>
+      <c r="C96" s="1">
+        <v>1</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" s="3" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C98" s="1">
         <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C99" s="1">
-        <v>1</v>
+        <v>130</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C101" s="1">
-        <v>1</v>
+        <v>132</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="3" t="s">
-        <v>134</v>
+        <v>119</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>118</v>
+        <v>259</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C105" s="1">
         <v>1</v>
       </c>
-      <c r="D105" s="1" t="s">
-        <v>262</v>
+      <c r="D105" t="s">
+        <v>106</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>263</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C106" s="1">
-        <v>1</v>
-      </c>
-      <c r="D106" t="s">
-        <v>108</v>
+        <v>218</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>172</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>231</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B109" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B110" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C111" s="1">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="3" t="s">
-        <v>124</v>
+        <v>73</v>
+      </c>
+      <c r="C112" s="1">
+        <v>1</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B113" s="3" t="s">
-        <v>73</v>
+        <v>257</v>
       </c>
       <c r="C113" s="1">
         <v>1</v>
@@ -2714,89 +2697,93 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C114" s="1">
         <v>1</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B115" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C115" s="1">
-        <v>1</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>52</v>
+      <c r="A115" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>141</v>
+      <c r="B116" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="3" t="s">
-        <v>142</v>
+        <v>268</v>
       </c>
       <c r="C117" s="1">
         <v>1</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C119" s="1"/>
+        <v>174</v>
+      </c>
+      <c r="C119" s="1">
+        <v>1</v>
+      </c>
       <c r="D119" s="1" t="s">
-        <v>294</v>
+        <v>41</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C120" s="1"/>
+        <v>294</v>
+      </c>
+      <c r="C120" s="1">
+        <v>1</v>
+      </c>
       <c r="D120" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B121" s="3" t="s">
-        <v>176</v>
+        <v>295</v>
+      </c>
+      <c r="C121" s="1">
+        <v>1</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -2806,35 +2793,38 @@
       <c r="D122" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>296</v>
-      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
+      </c>
+      <c r="C123" s="1">
+        <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
+      </c>
+      <c r="C124" s="1">
+        <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -2845,7 +2835,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -2856,7 +2846,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -2867,7 +2857,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
@@ -2878,7 +2868,7 @@
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C129" s="1">
         <v>0.8</v>
@@ -2887,12 +2877,12 @@
         <v>41</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
@@ -2903,7 +2893,7 @@
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
@@ -2912,12 +2902,12 @@
         <v>41</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -2926,12 +2916,12 @@
         <v>41</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
@@ -2940,26 +2930,26 @@
         <v>41</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C134" s="1">
+        <v>1</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F134" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="C134" s="1">
-        <v>1</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F134" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C135" s="1">
         <v>0.8</v>
@@ -2968,12 +2958,12 @@
         <v>41</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C136" s="1">
         <v>1</v>
@@ -2982,40 +2972,40 @@
         <v>41</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C137" s="1">
         <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C138" s="1">
         <v>1</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C139" s="1">
         <v>1</v>
@@ -3024,26 +3014,26 @@
         <v>41</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C140" s="1">
         <v>1</v>
       </c>
       <c r="D140" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F140" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C141" s="1">
         <v>1</v>
@@ -3052,37 +3042,37 @@
         <v>41</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C142" s="1">
         <v>1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>41</v>
@@ -3090,67 +3080,67 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B145" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B146" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B147" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C147" s="1">
         <v>1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B148" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B149" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B150" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
@@ -3173,7 +3163,7 @@
         <v>52</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
@@ -3184,7 +3174,7 @@
         <v>52</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
@@ -3238,13 +3228,13 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C161" s="3"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C162">
         <f>COUNTA($D$2:$D$160)-COUNTIF($D$2:$D$160, "Deprecated")</f>
@@ -3253,20 +3243,20 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C163">
         <f>COUNTA($C$2:$C$160)</f>
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C164" s="12">
         <f>(C163/C162)</f>
-        <v>0.35606060606060608</v>
+        <v>0.40151515151515149</v>
       </c>
     </row>
   </sheetData>
@@ -3298,69 +3288,69 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="13" t="s">
         <v>217</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D2" t="s">
         <v>90</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
         <v>216</v>
-      </c>
-      <c r="D3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" t="s">
         <v>216</v>
-      </c>
-      <c r="D4" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D5" t="s">
         <v>90</v>
@@ -3368,7 +3358,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B6" s="5">
         <v>29</v>
@@ -3379,69 +3369,69 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="s">
         <v>216</v>
-      </c>
-      <c r="D7" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8" s="5"/>
       <c r="D8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D12" t="s">
         <v>90</v>
@@ -3449,10 +3439,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D13" t="s">
         <v>90</v>
@@ -3460,189 +3450,189 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D14" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D25" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D26" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D27" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D30" t="s">
         <v>90</v>
@@ -3679,48 +3669,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>225</v>
-      </c>
       <c r="C2" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="s">
         <v>216</v>
-      </c>
-      <c r="D2" t="s">
-        <v>218</v>
       </c>
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
         <v>216</v>
-      </c>
-      <c r="D3" t="s">
-        <v>218</v>
       </c>
       <c r="E3" s="11"/>
     </row>

</xml_diff>

<commit_message>
Implemented Expand command, Command Method name refactored
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5175"/>
@@ -1597,8 +1597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1683,6 +1683,9 @@
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>41</v>
       </c>
@@ -3247,7 +3250,7 @@
       </c>
       <c r="C163">
         <f>COUNTA($C$2:$C$160)</f>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -3256,7 +3259,7 @@
       </c>
       <c r="C164" s="12">
         <f>(C163/C162)</f>
-        <v>0.40151515151515149</v>
+        <v>0.40909090909090912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Command WebGet implemented and now being tested
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="298">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1160,6 +1160,10 @@
   </si>
   <si>
     <t>Wildcard supported in &lt;DirPath&gt;, FAST option deprecated</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASK, TIMEOUT deprecated, Added SHA hash support</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1605,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1813,7 +1817,10 @@
         <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>52</v>
+        <v>154</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fix WebGet hash bug
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="5175"/>
   </bookViews>
@@ -211,10 +211,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>New</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Need test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1164,6 +1160,10 @@
   </si>
   <si>
     <t>ASK, TIMEOUT deprecated, Added SHA hash support</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1609,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1628,7 +1628,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>20</v>
@@ -1637,7 +1637,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>36</v>
@@ -1684,7 +1684,7 @@
         <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1698,7 +1698,7 @@
         <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1752,7 +1752,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1788,11 +1788,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1808,27 +1808,30 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1858,7 +1861,7 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1873,15 +1876,15 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
-        <v>47</v>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1889,7 +1892,7 @@
         <v>46</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>297</v>
       </c>
       <c r="E23" s="1"/>
     </row>
@@ -1971,11 +1974,11 @@
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1983,10 +1986,10 @@
         <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1994,10 +1997,10 @@
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2005,10 +2008,10 @@
         <v>26</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2016,10 +2019,10 @@
         <v>27</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2036,18 +2039,18 @@
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2055,7 +2058,7 @@
         <v>31</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2063,7 +2066,7 @@
         <v>32</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2071,7 +2074,7 @@
         <v>33</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2079,7 +2082,7 @@
         <v>34</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2087,7 +2090,7 @@
         <v>35</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2099,64 +2102,64 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2168,107 +2171,107 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="F64" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2280,247 +2283,247 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B72" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B73" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B75" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B77" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B78" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B79" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.3">
@@ -2532,235 +2535,235 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C99" s="1">
         <v>1</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C100" s="1">
         <v>1</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B101" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B102" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C102" s="1">
         <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B103" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C103" s="1">
         <v>1</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B104" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C104" s="1">
         <v>1</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B105" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C106" s="1">
         <v>1</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B108" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C108" s="1">
         <v>1</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B109" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C109" s="1">
         <v>1</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B110" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C110" s="1">
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B111" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C111" s="1">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B112" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B113" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B114" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B115" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B116" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C116" s="1">
         <v>1</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B117" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B118" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C118" s="1">
         <v>1</v>
@@ -2771,7 +2774,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B119" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C119" s="1">
         <v>1</v>
@@ -2782,13 +2785,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B120" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C120" s="1">
         <v>1</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -2801,26 +2804,26 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B123" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C123" s="1">
         <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B124" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
@@ -2831,7 +2834,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B125" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C125" s="1">
         <v>1</v>
@@ -2840,12 +2843,12 @@
         <v>41</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B126" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C126" s="1">
         <v>1</v>
@@ -2854,12 +2857,12 @@
         <v>41</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B127" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
@@ -2870,54 +2873,54 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B128" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C128" s="1">
         <v>1</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B129" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B130" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C130" s="1">
         <v>1</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B131" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C131" s="1">
         <v>1</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B132" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C132" s="1">
         <v>1</v>
@@ -2928,7 +2931,7 @@
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B133" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C133" s="1">
         <v>1</v>
@@ -2939,7 +2942,7 @@
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B134" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C134" s="1">
         <v>1</v>
@@ -2950,7 +2953,7 @@
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B135" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C135" s="1">
         <v>1</v>
@@ -2961,7 +2964,7 @@
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B136" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C136" s="1">
         <v>0.8</v>
@@ -2970,12 +2973,12 @@
         <v>41</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C137" s="1">
         <v>1</v>
@@ -2986,7 +2989,7 @@
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B138" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C138" s="1">
         <v>1</v>
@@ -2995,12 +2998,12 @@
         <v>41</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B139" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C139" s="1">
         <v>1</v>
@@ -3009,12 +3012,12 @@
         <v>41</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C140" s="1">
         <v>1</v>
@@ -3023,12 +3026,12 @@
         <v>41</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C141" s="1">
         <v>1</v>
@@ -3037,12 +3040,12 @@
         <v>41</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C142" s="1">
         <v>0.8</v>
@@ -3051,12 +3054,12 @@
         <v>41</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B143" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C143" s="1">
         <v>1</v>
@@ -3065,40 +3068,40 @@
         <v>41</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B144" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C144" s="1">
         <v>1</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B145" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C145" s="1">
         <v>1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B146" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C146" s="1">
         <v>1</v>
@@ -3107,26 +3110,26 @@
         <v>41</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B147" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C147" s="1">
         <v>1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B148" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C148" s="1">
         <v>1</v>
@@ -3135,37 +3138,37 @@
         <v>41</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B149" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C149" s="1">
         <v>1</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B150" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B151" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>41</v>
@@ -3173,59 +3176,59 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B152" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B153" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B154" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C154" s="1">
         <v>1</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B155" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B156" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B157" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
@@ -3237,10 +3240,10 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
@@ -3251,76 +3254,76 @@
         <v>1</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E160" s="1"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B161" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B162" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B163" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C163" s="1">
         <v>1</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E163" s="1"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B164" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E164" s="1"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B165" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E165" s="1"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B166" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B167" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
@@ -3332,13 +3335,13 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C169" s="3"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C170">
         <f>COUNTA($D$2:$D$168)-COUNTIF($D$2:$D$168, "Deprecated")</f>
@@ -3347,20 +3350,20 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C171">
         <f>COUNTA($C$2:$C$168)</f>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C172" s="12">
         <f>(C171/C170)</f>
-        <v>0.45454545454545453</v>
+        <v>0.4621212121212121</v>
       </c>
     </row>
   </sheetData>
@@ -3392,354 +3395,354 @@
   <sheetData>
     <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>231</v>
-      </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>181</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>233</v>
-      </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B6" s="5">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>186</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" s="5"/>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>239</v>
-      </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>189</v>
-      </c>
       <c r="D14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="D15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>242</v>
-      </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>244</v>
-      </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>246</v>
-      </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>195</v>
-      </c>
       <c r="D20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>248</v>
-      </c>
       <c r="D21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>199</v>
-      </c>
       <c r="D23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>202</v>
-      </c>
       <c r="D25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="D26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>206</v>
-      </c>
       <c r="D27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>209</v>
-      </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -3773,48 +3776,48 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>212</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E3" s="11"/>
     </row>

</xml_diff>

<commit_message>
First commit of PEBakery.WPF, the GUI. Renamed PEBakery-Engine to PEBakery-Legacy. PEBakery-Legacy's part is re-assembled in the PEBakery-WPF.
</commit_message>
<xml_diff>
--- a/ResShare/SupportState.xlsx
+++ b/ResShare/SupportState.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="301">
   <si>
     <t>Registry</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1164,6 +1164,18 @@
   </si>
   <si>
     <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1610,7 +1622,7 @@
   <dimension ref="A1:F172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1683,6 +1695,9 @@
       <c r="D5" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E5" t="s">
+        <v>298</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1697,6 +1712,9 @@
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E6" t="s">
+        <v>300</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>295</v>
       </c>
@@ -1711,6 +1729,9 @@
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E7" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
@@ -1722,6 +1743,9 @@
       <c r="D8" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E8" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -1733,7 +1757,9 @@
       <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>48</v>
       </c>
@@ -1821,6 +1847,9 @@
       </c>
       <c r="D16" s="1" t="s">
         <v>153</v>
+      </c>
+      <c r="E16" t="s">
+        <v>299</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>296</v>

</xml_diff>